<commit_message>
Fix: added rolls in att-bulk-format
</commit_message>
<xml_diff>
--- a/erp/xlformats/attendance-bulk-format.xlsx
+++ b/erp/xlformats/attendance-bulk-format.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26903"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{236B08D6-84D3-4782-AA19-B22BB35806D9}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5DA127A-3C3D-42B4-9D69-7D2ABDB9B092}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,12 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Student Name</t>
   </si>
   <si>
     <t>Student ID</t>
+  </si>
+  <si>
+    <t>Class Roll</t>
+  </si>
+  <si>
+    <t>Univ Roll</t>
   </si>
   <si>
     <t>Prakhar Sinha</t>
@@ -408,66 +414,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
         <v>44740</v>
       </c>
-      <c r="D1" s="1">
+      <c r="F1" s="1">
         <v>44741</v>
       </c>
-      <c r="E1" s="2">
+      <c r="G1" s="2">
         <v>44742</v>
       </c>
-      <c r="F1" s="2">
+      <c r="H1" s="2">
         <v>44744</v>
       </c>
-      <c r="G1" s="2">
+      <c r="I1" s="2">
         <v>44745</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
+      <c r="I3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>